<commit_message>
fix some bugs; add random
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyulu\Documents\thesis\HRC_taskAlloc_w.TB_w.AR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B3B499-B226-4D0F-8F08-1E9E7FED1E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7848F967-C320-4803-82BB-7C9B9512605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23715" yWindow="11835" windowWidth="16200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>J1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,13 +58,35 @@
   <si>
     <t>Order</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t> J4  </t>
+  </si>
+  <si>
+    <t> J5  </t>
+  </si>
+  <si>
+    <t> J6  </t>
+  </si>
+  <si>
+    <t>J7  </t>
+  </si>
+  <si>
+    <t>J8  </t>
+  </si>
+  <si>
+    <t>J9  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +100,12 @@
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,8 +128,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -382,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -406,49 +440,151 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>36</v>
-      </c>
-      <c r="C2">
-        <v>54</v>
-      </c>
-      <c r="D2">
-        <v>36</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>72</v>
-      </c>
-      <c r="C3">
-        <v>70</v>
-      </c>
-      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>91</v>
+      </c>
+      <c r="C4" s="1">
+        <v>85</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>80</v>
-      </c>
-      <c r="C4">
+      <c r="B5" s="1">
+        <v>81</v>
+      </c>
+      <c r="C5" s="1">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>84</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1">
         <v>86</v>
       </c>
-      <c r="D4">
-        <v>78</v>
-      </c>
+      <c r="D9" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>76</v>
+      </c>
+      <c r="C10" s="1">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
get process time from therblig
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -1,33 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyulu\Documents\thesis\HRC_taskAlloc_w.TB_w.AR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Document\NTHU\master\HRC_taskalloc_w.TB_w.AR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4564FE5D-26D3-4B17-81BC-BD6DB3635E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A03E708-CE25-4896-8AD5-006C00C9B757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="8130" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32625" yWindow="3750" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processing Time" sheetId="1" r:id="rId1"/>
     <sheet name="Agents Sequence" sheetId="2" r:id="rId2"/>
-    <sheet name="Therblig Process Time" sheetId="3" r:id="rId3"/>
+    <sheet name="Chart1" sheetId="4" r:id="rId3"/>
+    <sheet name="Therblig Process Time" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>J1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,6 +120,10 @@
   </si>
   <si>
     <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Therblig</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -157,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +181,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -180,6 +197,1109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Therblig Process Time'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Therblig Process Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>TE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RL</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Therblig Process Time'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8B45-4D4B-9416-DBC59B03AAFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Therblig Process Time'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Therblig Process Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>TE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RL</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Therblig Process Time'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8B45-4D4B-9416-DBC59B03AAFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Therblig Process Time'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BOT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Therblig Process Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>TE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RL</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Therblig Process Time'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8B45-4D4B-9416-DBC59B03AAFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="456839295"/>
+        <c:axId val="456837375"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="456839295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456837375"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="456837375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456839295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{ED2E472C-15FF-4308-94DB-AEED62061892}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B89AF03-660D-D04E-4ED8-7D6E98F2E2BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -694,12 +1814,18 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -714,98 +1840,98 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
-        <v>34</v>
-      </c>
-      <c r="C2">
-        <v>33</v>
-      </c>
-      <c r="D2">
-        <v>44</v>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>40</v>
-      </c>
-      <c r="C3">
-        <v>39</v>
-      </c>
-      <c r="D3">
-        <v>44</v>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>22</v>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>22</v>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
-        <v>56</v>
-      </c>
-      <c r="C6">
-        <v>55</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7">
-        <v>106</v>
-      </c>
-      <c r="C7">
-        <v>105</v>
-      </c>
-      <c r="D7">
-        <v>110</v>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8">
-        <v>106</v>
-      </c>
-      <c r="C8">
-        <v>105</v>
-      </c>
-      <c r="D8">
-        <v>110</v>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>